<commit_message>
Update the data files with the national column
</commit_message>
<xml_diff>
--- a/data-wrangling/test/tiny-sample.xlsx
+++ b/data-wrangling/test/tiny-sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="599" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="SCHOOLS" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,27 +14,33 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ORGS!$A$1:$AK$10</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SCHOOLS!$A$2:$AW$10</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ORGS!$A$1:$AK$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ORGS!$A$1:$AK$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ORGS!$A$1:$AK$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ORGS!$A$1:$AK$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">GRANTS!$A$1:$S$541</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ORGS!$A$1:$AL$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8157" uniqueCount="3584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8162" uniqueCount="3585">
   <si>
     <t>Last 5 Years</t>
   </si>
@@ -10331,6 +10337,9 @@
     <t>Organization_name</t>
   </si>
   <si>
+    <t>National</t>
+  </si>
+  <si>
     <t>Location_of_services</t>
   </si>
   <si>
@@ -10410,6 +10419,9 @@
   </si>
   <si>
     <t>datetimelastupdated</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Bronx,Brooklyn,Manhattan,Queens,Greater New York,Outside NYC</t>
@@ -10439,9 +10451,6 @@
   </si>
   <si>
     <t>Nan Dale</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>A gift of $50.00 will help pay for the 30-day plumpy'nut treatment that Nico received in an Action Against Hunger health center.</t>
@@ -11082,9 +11091,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="\$#,##0.00" numFmtId="165"/>
+    <numFmt formatCode="@" numFmtId="166"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -11385,7 +11395,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -11570,6 +11580,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -43424,15 +43438,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ11"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A10" xSplit="0" ySplit="1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A11" activeCellId="0" pane="bottomLeft" sqref="A11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+      <selection activeCell="G7" activeCellId="0" pane="bottomLeft" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7091836734694"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.280612244898"/>
@@ -43440,16 +43454,16 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5714285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.28571428571429"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.0051020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.4234693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="28.9948979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.7142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5714285714286"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="35" min="16" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="21.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="44" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="39.0051020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2908163265306"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4234693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="28.9948979591837"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.7142857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.5714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.8571428571429"/>
+    <col collapsed="false" hidden="false" max="36" min="17" style="0" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="44" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="1">
@@ -43487,10 +43501,10 @@
         <v>3374</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>3375</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>3375</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>3376</v>
@@ -43532,10 +43546,10 @@
         <v>3388</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>3389</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>3389</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>3390</v>
@@ -43555,9 +43569,12 @@
       <c r="AH1" s="3" t="s">
         <v>3395</v>
       </c>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>3396</v>
+      </c>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3" t="s">
+        <v>3397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="2">
@@ -43579,47 +43596,47 @@
       <c r="F2" s="45" t="s">
         <v>543</v>
       </c>
-      <c r="G2" s="45" t="s">
-        <v>3397</v>
+      <c r="G2" s="46" t="s">
+        <v>3398</v>
       </c>
       <c r="H2" s="45" t="s">
+        <v>3399</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>3400</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>2608</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>3401</v>
+      </c>
+      <c r="L2" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>2604</v>
+      </c>
+      <c r="N2" s="45" t="s">
+        <v>3402</v>
+      </c>
+      <c r="O2" s="45" t="s">
+        <v>3403</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>3404</v>
+      </c>
+      <c r="Q2" s="45" t="s">
         <v>3398</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>2608</v>
-      </c>
-      <c r="J2" s="45" t="s">
-        <v>3399</v>
-      </c>
-      <c r="K2" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="45" t="s">
-        <v>2604</v>
-      </c>
-      <c r="M2" s="45" t="s">
-        <v>3400</v>
-      </c>
-      <c r="N2" s="45" t="s">
-        <v>3401</v>
-      </c>
-      <c r="O2" s="45" t="s">
-        <v>3402</v>
-      </c>
-      <c r="P2" s="45" t="s">
-        <v>3403</v>
-      </c>
-      <c r="Q2" s="45" t="s">
-        <v>3404</v>
       </c>
       <c r="R2" s="45" t="s">
         <v>3405</v>
       </c>
       <c r="S2" s="45" t="s">
-        <v>3403</v>
+        <v>3406</v>
       </c>
       <c r="T2" s="45" t="s">
-        <v>3406</v>
+        <v>3398</v>
       </c>
       <c r="U2" s="45" t="s">
         <v>3407</v>
@@ -43630,10 +43647,10 @@
       <c r="W2" s="45" t="s">
         <v>3409</v>
       </c>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45" t="s">
+      <c r="X2" s="45" t="s">
         <v>3410</v>
       </c>
+      <c r="Y2" s="45"/>
       <c r="Z2" s="45" t="s">
         <v>3411</v>
       </c>
@@ -43661,20 +43678,23 @@
       <c r="AH2" s="45" t="s">
         <v>3419</v>
       </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45" t="n">
+      <c r="AI2" s="45" t="s">
+        <v>3420</v>
+      </c>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45" t="n">
         <v>41331.415775463</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="3">
       <c r="A3" s="45" t="s">
-        <v>3420</v>
+        <v>3421</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>2611</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>3421</v>
+        <v>3422</v>
       </c>
       <c r="D3" s="45" t="s">
         <v>110</v>
@@ -43685,23 +43705,21 @@
       <c r="F3" s="45" t="s">
         <v>1503</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>3398</v>
-      </c>
+      <c r="G3" s="46"/>
       <c r="H3" s="45" t="s">
-        <v>3398</v>
+        <v>3400</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>3422</v>
+        <v>3400</v>
       </c>
       <c r="J3" s="45" t="s">
         <v>3423</v>
       </c>
       <c r="K3" s="45" t="s">
+        <v>3424</v>
+      </c>
+      <c r="L3" s="45" t="s">
         <v>119</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>3424</v>
       </c>
       <c r="M3" s="45" t="s">
         <v>3425</v>
@@ -43713,19 +43731,19 @@
         <v>3427</v>
       </c>
       <c r="P3" s="45" t="s">
-        <v>3403</v>
+        <v>3428</v>
       </c>
       <c r="Q3" s="45" t="s">
-        <v>3428</v>
+        <v>3398</v>
       </c>
       <c r="R3" s="45" t="s">
         <v>3429</v>
       </c>
       <c r="S3" s="45" t="s">
-        <v>3403</v>
+        <v>3430</v>
       </c>
       <c r="T3" s="45" t="s">
-        <v>3430</v>
+        <v>3398</v>
       </c>
       <c r="U3" s="45" t="s">
         <v>3431</v>
@@ -43734,10 +43752,10 @@
         <v>3432</v>
       </c>
       <c r="W3" s="45" t="s">
-        <v>3409</v>
+        <v>3433</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>3433</v>
+        <v>3410</v>
       </c>
       <c r="Y3" s="45" t="s">
         <v>3434</v>
@@ -43752,14 +43770,14 @@
         <v>3437</v>
       </c>
       <c r="AC3" s="45" t="s">
+        <v>3438</v>
+      </c>
+      <c r="AD3" s="45" t="s">
         <v>2615</v>
       </c>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45" t="s">
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="45" t="s">
         <v>2616</v>
-      </c>
-      <c r="AF3" s="45" t="s">
-        <v>3438</v>
       </c>
       <c r="AG3" s="45" t="s">
         <v>3439</v>
@@ -43767,20 +43785,23 @@
       <c r="AH3" s="45" t="s">
         <v>3440</v>
       </c>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45" t="n">
+      <c r="AI3" s="45" t="s">
+        <v>3441</v>
+      </c>
+      <c r="AJ3" s="45"/>
+      <c r="AK3" s="45" t="n">
         <v>41340.728912037</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="4">
       <c r="A4" s="45" t="s">
-        <v>3441</v>
+        <v>3442</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>3442</v>
+        <v>3443</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>3443</v>
+        <v>3444</v>
       </c>
       <c r="D4" s="45" t="s">
         <v>110</v>
@@ -43789,25 +43810,23 @@
         <v>37</v>
       </c>
       <c r="F4" s="45" t="s">
-        <v>3444</v>
-      </c>
-      <c r="G4" s="45" t="s">
-        <v>110</v>
-      </c>
+        <v>3445</v>
+      </c>
+      <c r="G4" s="46"/>
       <c r="H4" s="45" t="s">
         <v>110</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>3445</v>
+        <v>110</v>
       </c>
       <c r="J4" s="45" t="s">
         <v>3446</v>
       </c>
       <c r="K4" s="45" t="s">
+        <v>3447</v>
+      </c>
+      <c r="L4" s="45" t="s">
         <v>119</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>3447</v>
       </c>
       <c r="M4" s="45" t="s">
         <v>3448</v>
@@ -43819,26 +43838,26 @@
         <v>3450</v>
       </c>
       <c r="P4" s="45" t="s">
-        <v>3403</v>
+        <v>3451</v>
       </c>
       <c r="Q4" s="45" t="s">
-        <v>3451</v>
+        <v>3398</v>
       </c>
       <c r="R4" s="45" t="s">
         <v>3452</v>
       </c>
       <c r="S4" s="45" t="s">
-        <v>3403</v>
+        <v>3453</v>
       </c>
       <c r="T4" s="45" t="s">
-        <v>3453</v>
-      </c>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45" t="s">
-        <v>3408</v>
-      </c>
+        <v>3398</v>
+      </c>
+      <c r="U4" s="45" t="s">
+        <v>3454</v>
+      </c>
+      <c r="V4" s="45"/>
       <c r="W4" s="45" t="s">
-        <v>3454</v>
+        <v>3409</v>
       </c>
       <c r="X4" s="45" t="s">
         <v>3455</v>
@@ -43858,83 +43877,84 @@
       <c r="AC4" s="45" t="s">
         <v>3460</v>
       </c>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="45" t="s">
+      <c r="AD4" s="45" t="s">
         <v>3461</v>
       </c>
+      <c r="AE4" s="45"/>
       <c r="AF4" s="45" t="s">
         <v>3462</v>
       </c>
       <c r="AG4" s="45" t="s">
-        <v>3390</v>
+        <v>3463</v>
       </c>
       <c r="AH4" s="45" t="s">
-        <v>3463</v>
-      </c>
-      <c r="AI4" s="45"/>
-      <c r="AJ4" s="45" t="n">
+        <v>3391</v>
+      </c>
+      <c r="AI4" s="45" t="s">
+        <v>3464</v>
+      </c>
+      <c r="AJ4" s="45"/>
+      <c r="AK4" s="45" t="n">
         <v>41593.6048032407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="5">
       <c r="A5" s="45" t="s">
-        <v>3464</v>
+        <v>3465</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>3465</v>
+        <v>3466</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>3466</v>
+        <v>3467</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>3467</v>
+        <v>3468</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>3468</v>
-      </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45" t="s">
         <v>3469</v>
       </c>
+      <c r="G5" s="46"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="45" t="s">
         <v>3470</v>
       </c>
       <c r="J5" s="45" t="s">
         <v>3471</v>
       </c>
-      <c r="K5" s="45"/>
+      <c r="K5" s="45" t="s">
+        <v>3472</v>
+      </c>
       <c r="L5" s="45"/>
-      <c r="M5" s="45" t="s">
-        <v>3472</v>
-      </c>
+      <c r="M5" s="45"/>
       <c r="N5" s="45" t="s">
-        <v>3449</v>
+        <v>3473</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>3473</v>
+        <v>3450</v>
       </c>
       <c r="P5" s="45" t="s">
-        <v>3403</v>
+        <v>3474</v>
       </c>
       <c r="Q5" s="45" t="s">
-        <v>3474</v>
+        <v>3398</v>
       </c>
       <c r="R5" s="45" t="s">
         <v>3475</v>
       </c>
       <c r="S5" s="45" t="s">
-        <v>3403</v>
+        <v>3476</v>
       </c>
       <c r="T5" s="45" t="s">
-        <v>3476</v>
-      </c>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45" t="s">
+        <v>3398</v>
+      </c>
+      <c r="U5" s="45" t="s">
         <v>3477</v>
       </c>
+      <c r="V5" s="45"/>
       <c r="W5" s="45" t="s">
         <v>3478</v>
       </c>
@@ -43956,19 +43976,22 @@
       <c r="AC5" s="45" t="s">
         <v>3484</v>
       </c>
-      <c r="AD5" s="45"/>
+      <c r="AD5" s="45" t="s">
+        <v>3485</v>
+      </c>
       <c r="AE5" s="45"/>
-      <c r="AF5" s="45" t="s">
-        <v>3485</v>
-      </c>
+      <c r="AF5" s="45"/>
       <c r="AG5" s="45" t="s">
-        <v>3418</v>
+        <v>3486</v>
       </c>
       <c r="AH5" s="45" t="s">
         <v>3419</v>
       </c>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="45" t="n">
+      <c r="AI5" s="45" t="s">
+        <v>3420</v>
+      </c>
+      <c r="AJ5" s="45"/>
+      <c r="AK5" s="45" t="n">
         <v>40700.3307523148</v>
       </c>
     </row>
@@ -43991,11 +44014,11 @@
       <c r="F6" s="45" t="s">
         <v>1302</v>
       </c>
-      <c r="G6" s="45" t="s">
-        <v>3486</v>
+      <c r="G6" s="46" t="s">
+        <v>3398</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>3486</v>
+        <v>3487</v>
       </c>
       <c r="I6" s="45" t="s">
         <v>3487</v>
@@ -44004,13 +44027,13 @@
         <v>3488</v>
       </c>
       <c r="K6" s="45" t="s">
+        <v>3489</v>
+      </c>
+      <c r="L6" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="L6" s="45" t="s">
+      <c r="M6" s="45" t="s">
         <v>1299</v>
-      </c>
-      <c r="M6" s="45" t="s">
-        <v>3489</v>
       </c>
       <c r="N6" s="45" t="s">
         <v>3490</v>
@@ -44019,34 +44042,34 @@
         <v>3491</v>
       </c>
       <c r="P6" s="45" t="s">
-        <v>3403</v>
+        <v>3492</v>
       </c>
       <c r="Q6" s="45" t="s">
-        <v>3492</v>
+        <v>3398</v>
       </c>
       <c r="R6" s="45" t="s">
         <v>3493</v>
       </c>
       <c r="S6" s="45" t="s">
-        <v>3403</v>
+        <v>3494</v>
       </c>
       <c r="T6" s="45" t="s">
-        <v>3494</v>
+        <v>3398</v>
       </c>
       <c r="U6" s="45" t="s">
         <v>3495</v>
       </c>
       <c r="V6" s="45" t="s">
-        <v>3408</v>
+        <v>3496</v>
       </c>
       <c r="W6" s="45" t="s">
-        <v>3496</v>
+        <v>3409</v>
       </c>
       <c r="X6" s="45" t="s">
-        <v>3455</v>
+        <v>3497</v>
       </c>
       <c r="Y6" s="45" t="s">
-        <v>3497</v>
+        <v>3456</v>
       </c>
       <c r="Z6" s="45" t="s">
         <v>3498</v>
@@ -44060,85 +44083,86 @@
       <c r="AC6" s="45" t="s">
         <v>3501</v>
       </c>
-      <c r="AD6" s="45"/>
+      <c r="AD6" s="45" t="s">
+        <v>3502</v>
+      </c>
       <c r="AE6" s="45"/>
-      <c r="AF6" s="45" t="s">
-        <v>3502</v>
-      </c>
+      <c r="AF6" s="45"/>
       <c r="AG6" s="45" t="s">
-        <v>3502</v>
+        <v>3503</v>
       </c>
       <c r="AH6" s="45" t="s">
-        <v>3419</v>
-      </c>
-      <c r="AI6" s="45"/>
-      <c r="AJ6" s="45" t="n">
+        <v>3503</v>
+      </c>
+      <c r="AI6" s="45" t="s">
+        <v>3420</v>
+      </c>
+      <c r="AJ6" s="45"/>
+      <c r="AK6" s="45" t="n">
         <v>41324.7414351852</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="7">
       <c r="A7" s="45" t="s">
-        <v>3503</v>
+        <v>3504</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>3504</v>
+        <v>3505</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>3505</v>
+        <v>3506</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>3506</v>
+        <v>3507</v>
       </c>
       <c r="E7" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>3507</v>
-      </c>
-      <c r="G7" s="45" t="s">
         <v>3508</v>
       </c>
+      <c r="G7" s="46"/>
       <c r="H7" s="45" t="s">
-        <v>3469</v>
+        <v>3509</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>3509</v>
+        <v>3470</v>
       </c>
       <c r="J7" s="45" t="s">
         <v>3510</v>
       </c>
       <c r="K7" s="45" t="s">
+        <v>3511</v>
+      </c>
+      <c r="L7" s="45" t="s">
         <v>229</v>
-      </c>
-      <c r="L7" s="45" t="s">
-        <v>3511</v>
       </c>
       <c r="M7" s="45" t="s">
         <v>3512</v>
       </c>
       <c r="N7" s="45" t="s">
-        <v>3449</v>
+        <v>3513</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>3513</v>
+        <v>3450</v>
       </c>
       <c r="P7" s="45" t="s">
-        <v>3403</v>
+        <v>3514</v>
       </c>
       <c r="Q7" s="45" t="s">
-        <v>3514</v>
-      </c>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45" t="s">
-        <v>3403</v>
-      </c>
+        <v>3398</v>
+      </c>
+      <c r="R7" s="45" t="s">
+        <v>3515</v>
+      </c>
+      <c r="S7" s="45"/>
       <c r="T7" s="45" t="s">
-        <v>3515</v>
-      </c>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45" t="s">
+        <v>3398</v>
+      </c>
+      <c r="U7" s="45" t="s">
         <v>3516</v>
       </c>
+      <c r="V7" s="45"/>
       <c r="W7" s="45" t="s">
         <v>3517</v>
       </c>
@@ -44152,18 +44176,18 @@
         <v>3520</v>
       </c>
       <c r="AA7" s="45" t="s">
-        <v>3458</v>
+        <v>3521</v>
       </c>
       <c r="AB7" s="45" t="s">
-        <v>3521</v>
+        <v>3459</v>
       </c>
       <c r="AC7" s="45" t="s">
         <v>3522</v>
       </c>
-      <c r="AD7" s="45"/>
-      <c r="AE7" s="45" t="s">
+      <c r="AD7" s="45" t="s">
         <v>3523</v>
       </c>
+      <c r="AE7" s="45"/>
       <c r="AF7" s="45" t="s">
         <v>3524</v>
       </c>
@@ -44173,8 +44197,11 @@
       <c r="AH7" s="45" t="s">
         <v>3526</v>
       </c>
-      <c r="AI7" s="45"/>
-      <c r="AJ7" s="45" t="n">
+      <c r="AI7" s="45" t="s">
+        <v>3527</v>
+      </c>
+      <c r="AJ7" s="45"/>
+      <c r="AK7" s="45" t="n">
         <v>40855.6934143519</v>
       </c>
     </row>
@@ -44197,48 +44224,48 @@
       <c r="F8" s="45" t="s">
         <v>1314</v>
       </c>
-      <c r="G8" s="45"/>
+      <c r="G8" s="46" t="s">
+        <v>3398</v>
+      </c>
       <c r="H8" s="45"/>
-      <c r="I8" s="45" t="s">
-        <v>3527</v>
-      </c>
+      <c r="I8" s="45"/>
       <c r="J8" s="45" t="s">
         <v>3528</v>
       </c>
       <c r="K8" s="45" t="s">
+        <v>3529</v>
+      </c>
+      <c r="L8" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="45" t="s">
+      <c r="M8" s="45" t="s">
         <v>1310</v>
       </c>
-      <c r="M8" s="45" t="s">
-        <v>3529</v>
-      </c>
       <c r="N8" s="45" t="s">
-        <v>3449</v>
+        <v>3530</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>3530</v>
+        <v>3450</v>
       </c>
       <c r="P8" s="45" t="s">
         <v>3531</v>
       </c>
-      <c r="Q8" s="45"/>
+      <c r="Q8" s="45" t="s">
+        <v>3532</v>
+      </c>
       <c r="R8" s="45"/>
-      <c r="S8" s="45" t="s">
-        <v>3403</v>
-      </c>
+      <c r="S8" s="45"/>
       <c r="T8" s="45" t="s">
-        <v>3532</v>
+        <v>3398</v>
       </c>
       <c r="U8" s="45" t="s">
         <v>3533</v>
       </c>
       <c r="V8" s="45" t="s">
-        <v>3408</v>
+        <v>3534</v>
       </c>
       <c r="W8" s="45" t="s">
-        <v>3534</v>
+        <v>3409</v>
       </c>
       <c r="X8" s="45" t="s">
         <v>3535</v>
@@ -44258,19 +44285,22 @@
       <c r="AC8" s="45" t="s">
         <v>3540</v>
       </c>
-      <c r="AD8" s="45"/>
+      <c r="AD8" s="45" t="s">
+        <v>3541</v>
+      </c>
       <c r="AE8" s="45"/>
-      <c r="AF8" s="45" t="s">
-        <v>3541</v>
-      </c>
+      <c r="AF8" s="45"/>
       <c r="AG8" s="45" t="s">
         <v>3542</v>
       </c>
       <c r="AH8" s="45" t="s">
         <v>3543</v>
       </c>
-      <c r="AI8" s="45"/>
-      <c r="AJ8" s="45" t="n">
+      <c r="AI8" s="45" t="s">
+        <v>3544</v>
+      </c>
+      <c r="AJ8" s="45"/>
+      <c r="AK8" s="45" t="n">
         <v>40592.5803703704</v>
       </c>
     </row>
@@ -44293,26 +44323,24 @@
       <c r="F9" s="45" t="s">
         <v>864</v>
       </c>
-      <c r="G9" s="45" t="s">
-        <v>3544</v>
-      </c>
+      <c r="G9" s="46"/>
       <c r="H9" s="45" t="s">
+        <v>3545</v>
+      </c>
+      <c r="I9" s="45" t="s">
         <v>2843</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="J9" s="45" t="s">
         <v>3126</v>
       </c>
-      <c r="J9" s="45" t="s">
-        <v>3545</v>
-      </c>
       <c r="K9" s="45" t="s">
+        <v>3546</v>
+      </c>
+      <c r="L9" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="L9" s="45" t="s">
+      <c r="M9" s="45" t="s">
         <v>3121</v>
-      </c>
-      <c r="M9" s="45" t="s">
-        <v>3546</v>
       </c>
       <c r="N9" s="45" t="s">
         <v>3547</v>
@@ -44321,19 +44349,19 @@
         <v>3548</v>
       </c>
       <c r="P9" s="45" t="s">
-        <v>3403</v>
+        <v>3549</v>
       </c>
       <c r="Q9" s="45" t="s">
-        <v>3549</v>
+        <v>3398</v>
       </c>
       <c r="R9" s="45" t="s">
         <v>3550</v>
       </c>
       <c r="S9" s="45" t="s">
-        <v>3403</v>
+        <v>3551</v>
       </c>
       <c r="T9" s="45" t="s">
-        <v>3551</v>
+        <v>3398</v>
       </c>
       <c r="U9" s="45" t="s">
         <v>3552</v>
@@ -44360,16 +44388,16 @@
         <v>3559</v>
       </c>
       <c r="AC9" s="45" t="s">
+        <v>3560</v>
+      </c>
+      <c r="AD9" s="45" t="s">
         <v>3124</v>
       </c>
-      <c r="AD9" s="45" t="s">
-        <v>3560</v>
-      </c>
       <c r="AE9" s="45" t="s">
+        <v>3561</v>
+      </c>
+      <c r="AF9" s="45" t="s">
         <v>3125</v>
-      </c>
-      <c r="AF9" s="45" t="s">
-        <v>3561</v>
       </c>
       <c r="AG9" s="45" t="s">
         <v>3562</v>
@@ -44377,20 +44405,23 @@
       <c r="AH9" s="45" t="s">
         <v>3563</v>
       </c>
-      <c r="AI9" s="45"/>
-      <c r="AJ9" s="45" t="n">
+      <c r="AI9" s="45" t="s">
+        <v>3564</v>
+      </c>
+      <c r="AJ9" s="45"/>
+      <c r="AK9" s="45" t="n">
         <v>41313.4423148148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="10">
       <c r="A10" s="45" t="s">
-        <v>3564</v>
+        <v>3565</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>3565</v>
+        <v>3566</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>3566</v>
+        <v>3567</v>
       </c>
       <c r="D10" s="45" t="s">
         <v>597</v>
@@ -44399,59 +44430,59 @@
         <v>451</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>3567</v>
-      </c>
-      <c r="G10" s="45" t="s">
         <v>3568</v>
       </c>
+      <c r="G10" s="46" t="s">
+        <v>3398</v>
+      </c>
       <c r="H10" s="45" t="s">
-        <v>3486</v>
+        <v>3569</v>
       </c>
       <c r="I10" s="45" t="s">
+        <v>3487</v>
+      </c>
+      <c r="J10" s="45" t="s">
         <v>454</v>
       </c>
-      <c r="J10" s="45" t="s">
-        <v>3569</v>
-      </c>
-      <c r="K10" s="45"/>
+      <c r="K10" s="45" t="s">
+        <v>3570</v>
+      </c>
       <c r="L10" s="45"/>
-      <c r="M10" s="45" t="s">
-        <v>3570</v>
-      </c>
+      <c r="M10" s="45"/>
       <c r="N10" s="45" t="s">
-        <v>3449</v>
+        <v>3571</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>3571</v>
+        <v>3450</v>
       </c>
       <c r="P10" s="45" t="s">
-        <v>3403</v>
+        <v>3572</v>
       </c>
       <c r="Q10" s="45" t="s">
-        <v>3572</v>
+        <v>3398</v>
       </c>
       <c r="R10" s="45" t="s">
         <v>3573</v>
       </c>
       <c r="S10" s="45" t="s">
-        <v>3403</v>
+        <v>3574</v>
       </c>
       <c r="T10" s="45" t="s">
-        <v>3574</v>
+        <v>3398</v>
       </c>
       <c r="U10" s="45" t="s">
         <v>3575</v>
       </c>
       <c r="V10" s="45" t="s">
-        <v>3408</v>
+        <v>3576</v>
       </c>
       <c r="W10" s="45" t="s">
-        <v>3576</v>
-      </c>
-      <c r="X10" s="45"/>
-      <c r="Y10" s="45" t="s">
+        <v>3409</v>
+      </c>
+      <c r="X10" s="45" t="s">
         <v>3577</v>
       </c>
+      <c r="Y10" s="45"/>
       <c r="Z10" s="45" t="s">
         <v>3578</v>
       </c>
@@ -44464,25 +44495,27 @@
       <c r="AC10" s="45" t="s">
         <v>3581</v>
       </c>
-      <c r="AD10" s="45"/>
+      <c r="AD10" s="45" t="s">
+        <v>3582</v>
+      </c>
       <c r="AE10" s="45"/>
-      <c r="AF10" s="45" t="s">
-        <v>3582</v>
-      </c>
+      <c r="AF10" s="45"/>
       <c r="AG10" s="45" t="s">
-        <v>3418</v>
+        <v>3583</v>
       </c>
       <c r="AH10" s="45" t="s">
-        <v>3583</v>
-      </c>
-      <c r="AI10" s="45"/>
-      <c r="AJ10" s="45" t="n">
+        <v>3419</v>
+      </c>
+      <c r="AI10" s="45" t="s">
+        <v>3584</v>
+      </c>
+      <c r="AJ10" s="45"/>
+      <c r="AK10" s="45" t="n">
         <v>41436.5021296296</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11"/>
   </sheetData>
-  <autoFilter ref="A1:AK10"/>
+  <autoFilter ref="A1:AL10"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>